<commit_message>
fix qa errors to examples and CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
+++ b/input/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\input\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8D7DAF-9E94-4352-9F83-F8B4AC0BD1E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD08B8-DA36-49BC-BD57-1474494EB05C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-465" windowWidth="19440" windowHeight="15000" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-17790" yWindow="90" windowWidth="25200" windowHeight="13425" activeTab="1" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -475,9 +475,6 @@
     <t>canon</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/</t>
-  </si>
-  <si>
     <t>publisher</t>
   </si>
   <si>
@@ -513,6 +510,9 @@
   </si>
   <si>
     <t>For general security consideration refer to the [Security and Privacy Considerations](http://hl7.org/fhir/R4/secpriv-module.html).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/</t>
   </si>
 </sst>
 </file>
@@ -948,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -979,7 +979,7 @@
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +1019,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3541C921-3773-4F8B-BCA2-B06559AD2535}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,31 +1154,31 @@
         <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
         <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
         <v>135</v>
-      </c>
-      <c r="B7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
         <v>137</v>
-      </c>
-      <c r="B8" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1213,7 +1213,7 @@
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update version, fix file names
</commit_message>
<xml_diff>
--- a/input/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
+++ b/input/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\input\resources\source-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-DEQM/input/resources/source-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD08B8-DA36-49BC-BD57-1474494EB05C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463640FC-35A8-D24D-A1C5-113FC215EB02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17790" yWindow="90" windowWidth="25200" windowHeight="13425" activeTab="1" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-25200" yWindow="100" windowWidth="25200" windowHeight="13420" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -427,9 +427,6 @@
     <t>http://hl7.org/fhir/OperationDefinition/Measure-collect-data</t>
   </si>
   <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/devicerequest-deqm</t>
   </si>
   <si>
@@ -506,13 +503,16 @@
 </t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/ImplementationGuide/hl7.fhir.us.davinci-deqm|1.1.0</t>
-  </si>
-  <si>
     <t>For general security consideration refer to the [Security and Privacy Considerations](http://hl7.org/fhir/R4/secpriv-module.html).</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/davinci-deqm/</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/ImplementationGuide/hl7.fhir.us.davinci-deqm|2.0.0</t>
   </si>
 </sst>
 </file>
@@ -948,17 +948,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -966,23 +966,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -990,7 +990,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -998,15 +998,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1014,20 +1014,20 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1043,9 +1043,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1111,13 +1111,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3541C921-3773-4F8B-BCA2-B06559AD2535}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1125,60 +1125,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>129</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>131</v>
       </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>132</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>134</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1194,13 +1194,13 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="68.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1208,20 +1208,20 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1238,15 +1238,15 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.42578125" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="98.5" customWidth="1"/>
+    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1260,9 +1260,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -1274,9 +1274,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -1288,9 +1288,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -1302,9 +1302,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -1316,9 +1316,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
@@ -1330,9 +1330,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -1344,9 +1344,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
@@ -1358,9 +1358,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
@@ -1372,7 +1372,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -1405,19 +1405,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -1537,16 +1537,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1594,14 +1594,14 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1612,17 +1612,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1633,32 +1633,32 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1676,13 +1676,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -1742,21 +1742,21 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" customWidth="1"/>
+    <col min="9" max="15" width="9.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applied FHIR-37898 (changes affected many files) Reversed FHIR-32980 (changes to be re-applied in Jan2023 ballot) Deleted input/drafts folder (historical and no longer needed)
</commit_message>
<xml_diff>
--- a/input/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
+++ b/input/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-DEQM/input/resources/source-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\davinci-deqm\input\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463640FC-35A8-D24D-A1C5-113FC215EB02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4466DC2-74DE-4537-AE36-E7C459F32702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25200" yWindow="100" windowWidth="25200" windowHeight="13420" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="3312" yWindow="1020" windowWidth="26052" windowHeight="15240" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -259,9 +262,6 @@
     <t>DEQM DeviceUseStatement Profile</t>
   </si>
   <si>
-    <t>DEQM Organization Profile</t>
-  </si>
-  <si>
     <t>DEQM Coverage Profile</t>
   </si>
   <si>
@@ -442,9 +442,6 @@
     <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/deviceusestatement-deqm</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/organization-deqm</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/coverage-deqm</t>
   </si>
   <si>
@@ -491,12 +488,6 @@
   </si>
   <si>
     <t>4.0.1</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/qicore/ImplementationGuide/hl7.fhir.us.qicore|4.0.0</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/cqfmeasures/ImplementationGuide/hl7.fhir.us.cqfmeasures|2.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">Da Vinci DEQM Consumer Client **SHALL** support the Collect Data  transaction defined in the *Framework* Section of  this  Implementation Guide.
@@ -509,10 +500,22 @@
     <t>http://hl7.org/fhir/us/davinci-deqm/</t>
   </si>
   <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/ImplementationGuide/hl7.fhir.us.davinci-deqm|2.0.0</t>
+    <t>http://hl7.org/fhir/us/qicore/StructureDefinition/qicore-organization</t>
+  </si>
+  <si>
+    <t>QI Core Organization Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/qicore/ImplementationGuide/hl7.fhir.us.qicore|4.1.1</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/cqfmeasures/ImplementationGuide/hl7.fhir.us.cqfmeasures|3.0.0</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/ImplementationGuide/hl7.fhir.us.davinci-deqm|3.1.0</t>
   </si>
 </sst>
 </file>
@@ -952,13 +955,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -966,39 +969,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="80" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1006,28 +1009,28 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1043,59 +1046,59 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>110</v>
       </c>
       <c r="J2" s="7" t="str">
         <f t="shared" ref="J2" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
@@ -1115,9 +1118,9 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1125,60 +1128,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>124</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>126</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>128</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>131</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>133</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1191,37 +1194,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" customWidth="1"/>
     <col min="3" max="3" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" t="s">
-        <v>139</v>
+        <v>70</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1235,18 +1238,18 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="98.5" customWidth="1"/>
-    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="98.44140625" customWidth="1"/>
+    <col min="2" max="2" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1260,9 +1263,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -1274,9 +1277,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -1288,12 +1291,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1302,9 +1305,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -1316,9 +1319,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
@@ -1330,12 +1333,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>121</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1344,12 +1347,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>122</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1358,12 +1361,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1372,18 +1375,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
         <v>112</v>
-      </c>
-      <c r="B10" t="s">
-        <v>113</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1405,19 +1408,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1431,76 +1434,76 @@
         <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
         <v>37</v>
       </c>
       <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>80</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>81</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>82</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>83</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>84</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>85</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>86</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>87</v>
       </c>
       <c r="R1" t="s">
         <v>27</v>
       </c>
       <c r="S1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="X1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1508,12 +1511,12 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1537,16 +1540,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1563,18 +1566,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1594,71 +1597,71 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1676,13 +1679,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1690,42 +1693,42 @@
         <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>97</v>
       </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>98</v>
-      </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1742,21 +1745,21 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="5" width="9.109375" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="34.6640625" customWidth="1"/>
-    <col min="9" max="15" width="9.1640625" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
-    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="9.109375" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" customWidth="1"/>
+    <col min="17" max="17" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
     </row>
   </sheetData>

</xml_diff>